<commit_message>
multi jawaban + upload live
</commit_message>
<xml_diff>
--- a/assets/website/template/upload_soal/Template_upload_soal.xlsx
+++ b/assets/website/template/upload_soal/Template_upload_soal.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp\htdocs\cbt\assets\website\template\upload_soal\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\xampp\htdocs\cbt\assets\website\template\upload_soal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A22A6450-7284-428E-889E-158329E429D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85C75104-75F0-41CD-A400-7BC43DA47B6F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{3183A954-837B-4441-B86C-D9A4F25D3E5A}"/>
   </bookViews>
@@ -34,6 +34,7 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>candraajipamungkas</author>
+    <author>Candra</author>
   </authors>
   <commentList>
     <comment ref="A1" authorId="0" shapeId="0" xr:uid="{09425AD8-7547-4D9B-9E4E-5E5C0F24A57B}">
@@ -82,7 +83,7 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-Saat pengisian isi jawaban di kolom A - E, sesuaikan dengan mode jawaban anda, Jika anda memilih hanya sampai C maka D dan E dikosongkan, Harap tidak menghapus kolom karena akan berakibat fatal saat upload berlangsung</t>
+Saat pengisian isi jawaban di kolom A - J, sesuaikan dengan mode jawaban anda, Jika anda memilih hanya sampai C maka D dan E dikosongkan, Harap tidak menghapus kolom karena akan berakibat fatal saat upload berlangsung, Jika memilih jawaban multiple pisahkan jawaban kedua dengan koma tanpa spasi</t>
         </r>
       </text>
     </comment>
@@ -212,12 +213,85 @@
         </r>
       </text>
     </comment>
+    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{ACA97614-53F5-41BB-AD81-BD2D7B4179AC}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>candraajipamungkas:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Jika pakai opsi jawaban single isi dengan angka 1 jika pakai jawaban multiple isi dengan angka  2</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K1" authorId="1" shapeId="0" xr:uid="{3D9C7CE1-3897-4410-86B8-088D990BB004}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Candra:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Isi jawaban sesuai settingan jumlah opsi jawaban 
+paket soal</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="U1" authorId="1" shapeId="0" xr:uid="{D449571D-FD9D-487A-9A0A-38BDE8CE4224}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Candra:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Default isi 0, jangan dikosongi jika tidak diberi skor</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="53">
   <si>
     <t>Jenis Soal</t>
   </si>
@@ -288,31 +362,94 @@
     <t>SOAL bACAAN</t>
   </si>
   <si>
-    <t>ES</t>
-  </si>
-  <si>
-    <t>Upload Excel Essay</t>
-  </si>
-  <si>
     <t>Upload Excel PG</t>
   </si>
   <si>
-    <t>Excel Essay</t>
-  </si>
-  <si>
-    <t>Cara upload excel essay</t>
-  </si>
-  <si>
-    <t>Cara upload excel pilihan ganda</t>
-  </si>
-  <si>
     <t>www.pilihan-ganda.co</t>
   </si>
   <si>
-    <t>www.essay.co</t>
-  </si>
-  <si>
     <t>Excel Pilihan Ganda</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>Excel E</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>J</t>
+  </si>
+  <si>
+    <t>Opsi Jawaban</t>
+  </si>
+  <si>
+    <t>Excel F</t>
+  </si>
+  <si>
+    <t>Excel G</t>
+  </si>
+  <si>
+    <t>Excel H</t>
+  </si>
+  <si>
+    <t>Excel I</t>
+  </si>
+  <si>
+    <t>Excel J</t>
+  </si>
+  <si>
+    <t>C,F</t>
+  </si>
+  <si>
+    <t>Upload Excel PG 2</t>
+  </si>
+  <si>
+    <t>Excel Pilihan Ganda 2</t>
+  </si>
+  <si>
+    <t>Cara upload excel pilihan ganda Multiple</t>
+  </si>
+  <si>
+    <t>Cara upload excel pilihan ganda Single</t>
+  </si>
+  <si>
+    <t>Skor A</t>
+  </si>
+  <si>
+    <t>Skor B</t>
+  </si>
+  <si>
+    <t>Skor C</t>
+  </si>
+  <si>
+    <t>Skor D</t>
+  </si>
+  <si>
+    <t>Skor E</t>
+  </si>
+  <si>
+    <t>Skor F</t>
+  </si>
+  <si>
+    <t>Skor G</t>
+  </si>
+  <si>
+    <t>Skor H</t>
+  </si>
+  <si>
+    <t>Skor I</t>
+  </si>
+  <si>
+    <t>Skor J</t>
   </si>
 </sst>
 </file>
@@ -697,10 +834,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{136A4D57-86E0-48D7-9474-007534B7E398}">
-  <dimension ref="A1:P3"/>
+  <dimension ref="A1:AF3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -714,15 +851,20 @@
     <col min="7" max="7" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="7" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="7.28515625" customWidth="1"/>
+    <col min="19" max="19" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="30" width="6.7109375" customWidth="1"/>
+    <col min="31" max="31" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="37.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -751,39 +893,87 @@
         <v>8</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AE1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>16</v>
       </c>
       <c r="B2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" t="s">
         <v>25</v>
-      </c>
-      <c r="C2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" t="s">
-        <v>31</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -800,37 +990,91 @@
       <c r="I2">
         <v>0</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2">
+        <v>2</v>
+      </c>
+      <c r="K2" t="s">
         <v>18</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>19</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>20</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>21</v>
       </c>
-      <c r="O2" s="2" t="s">
-        <v>29</v>
+      <c r="O2" t="s">
+        <v>27</v>
       </c>
       <c r="P2" t="s">
-        <v>28</v>
+        <v>33</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>34</v>
+      </c>
+      <c r="R2" t="s">
+        <v>35</v>
+      </c>
+      <c r="S2" t="s">
+        <v>36</v>
+      </c>
+      <c r="T2" t="s">
+        <v>37</v>
+      </c>
+      <c r="U2">
+        <v>0</v>
+      </c>
+      <c r="V2">
+        <v>0</v>
+      </c>
+      <c r="W2">
+        <v>0</v>
+      </c>
+      <c r="X2">
+        <v>0</v>
+      </c>
+      <c r="Y2">
+        <v>0</v>
+      </c>
+      <c r="Z2">
+        <v>0</v>
+      </c>
+      <c r="AA2">
+        <v>0</v>
+      </c>
+      <c r="AB2">
+        <v>0</v>
+      </c>
+      <c r="AC2">
+        <v>0</v>
+      </c>
+      <c r="AD2">
+        <v>0</v>
+      </c>
+      <c r="AE2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="B3" t="s">
-        <v>24</v>
+        <v>39</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="E3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F3" t="s">
         <v>22</v>
@@ -844,17 +1088,65 @@
       <c r="I3">
         <v>0</v>
       </c>
-      <c r="O3" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="P3" t="s">
+      <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="K3" t="s">
+        <v>18</v>
+      </c>
+      <c r="L3" t="s">
+        <v>19</v>
+      </c>
+      <c r="M3" t="s">
+        <v>20</v>
+      </c>
+      <c r="N3" t="s">
+        <v>21</v>
+      </c>
+      <c r="O3" t="s">
         <v>27</v>
+      </c>
+      <c r="U3">
+        <v>0</v>
+      </c>
+      <c r="V3">
+        <v>0</v>
+      </c>
+      <c r="W3">
+        <v>0</v>
+      </c>
+      <c r="X3">
+        <v>0</v>
+      </c>
+      <c r="Y3">
+        <v>0</v>
+      </c>
+      <c r="Z3">
+        <v>0</v>
+      </c>
+      <c r="AA3">
+        <v>0</v>
+      </c>
+      <c r="AB3">
+        <v>0</v>
+      </c>
+      <c r="AC3">
+        <v>0</v>
+      </c>
+      <c r="AD3">
+        <v>0</v>
+      </c>
+      <c r="AE3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="AF3" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="O2" r:id="rId1" xr:uid="{9D8EBFFC-837C-4911-ACF2-697979B28303}"/>
-    <hyperlink ref="O3" r:id="rId2" xr:uid="{83E7A93D-976E-4851-B443-DFDE3FF8B530}"/>
+    <hyperlink ref="AE2" r:id="rId1" xr:uid="{9D8EBFFC-837C-4911-ACF2-697979B28303}"/>
+    <hyperlink ref="AE3" r:id="rId2" xr:uid="{8D632A28-6A4B-4F9D-B16A-16F2703A06D1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>

</xml_diff>